<commit_message>
#6 added id of an agent, added number of copies of agents
</commit_message>
<xml_diff>
--- a/colony.xlsx
+++ b/colony.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13485" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13485" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Environment_rules" sheetId="3" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="106">
   <si>
     <t>environment rows</t>
   </si>
@@ -270,9 +270,6 @@
     <t>u</t>
   </si>
   <si>
-    <t>e,e</t>
-  </si>
-  <si>
     <t>l</t>
   </si>
   <si>
@@ -285,9 +282,6 @@
     <t>&lt;&gt;</t>
   </si>
   <si>
-    <t>number of agents</t>
-  </si>
-  <si>
     <t>start i</t>
   </si>
   <si>
@@ -316,6 +310,36 @@
   </si>
   <si>
     <t>number of computational steps (-1 for infinite loop)</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>#</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Agent</t>
+  </si>
+  <si>
+    <t>number of copies (indexed from 0)</t>
+  </si>
+  <si>
+    <t>if the number of copies is greater than 1, then the id is formed from id underscore index</t>
+  </si>
+  <si>
+    <t>Agent2</t>
+  </si>
+  <si>
+    <t>Agent3</t>
+  </si>
+  <si>
+    <t>start I (-1 for random value)</t>
+  </si>
+  <si>
+    <t>start j (-1 for random value)</t>
   </si>
 </sst>
 </file>
@@ -636,9 +660,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -682,10 +704,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -720,17 +742,9 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
       <c r="B4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>97</v>
-      </c>
-      <c r="B5">
         <v>5</v>
       </c>
     </row>
@@ -741,10 +755,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:T24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:B10"/>
+      <selection activeCell="S19" sqref="S19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -973,6 +987,185 @@
         <v>76</v>
       </c>
     </row>
+    <row r="18" spans="8:20" x14ac:dyDescent="0.25">
+      <c r="H18" t="s">
+        <v>97</v>
+      </c>
+      <c r="I18" t="s">
+        <v>97</v>
+      </c>
+      <c r="J18" t="s">
+        <v>97</v>
+      </c>
+      <c r="K18" t="s">
+        <v>97</v>
+      </c>
+      <c r="L18" t="s">
+        <v>97</v>
+      </c>
+      <c r="M18" t="s">
+        <v>97</v>
+      </c>
+      <c r="N18" t="s">
+        <v>97</v>
+      </c>
+      <c r="R18" t="s">
+        <v>97</v>
+      </c>
+      <c r="S18" t="s">
+        <v>97</v>
+      </c>
+      <c r="T18" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="19" spans="8:20" x14ac:dyDescent="0.25">
+      <c r="H19" t="s">
+        <v>3</v>
+      </c>
+      <c r="I19" t="s">
+        <v>96</v>
+      </c>
+      <c r="J19" t="s">
+        <v>96</v>
+      </c>
+      <c r="K19" t="s">
+        <v>96</v>
+      </c>
+      <c r="L19" t="s">
+        <v>96</v>
+      </c>
+      <c r="M19" t="s">
+        <v>96</v>
+      </c>
+      <c r="N19" t="s">
+        <v>96</v>
+      </c>
+      <c r="R19" t="s">
+        <v>96</v>
+      </c>
+      <c r="S19" t="s">
+        <v>96</v>
+      </c>
+      <c r="T19" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="20" spans="8:20" x14ac:dyDescent="0.25">
+      <c r="H20" t="s">
+        <v>3</v>
+      </c>
+      <c r="I20" t="s">
+        <v>96</v>
+      </c>
+      <c r="J20" t="s">
+        <v>96</v>
+      </c>
+      <c r="K20" t="s">
+        <v>96</v>
+      </c>
+      <c r="L20" t="s">
+        <v>96</v>
+      </c>
+      <c r="M20" t="s">
+        <v>96</v>
+      </c>
+      <c r="N20" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="21" spans="8:20" x14ac:dyDescent="0.25">
+      <c r="H21" t="s">
+        <v>3</v>
+      </c>
+      <c r="I21" t="s">
+        <v>96</v>
+      </c>
+      <c r="J21" t="s">
+        <v>96</v>
+      </c>
+      <c r="K21" t="s">
+        <v>96</v>
+      </c>
+      <c r="L21" t="s">
+        <v>96</v>
+      </c>
+      <c r="M21" t="s">
+        <v>96</v>
+      </c>
+      <c r="N21" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="22" spans="8:20" x14ac:dyDescent="0.25">
+      <c r="H22" t="s">
+        <v>3</v>
+      </c>
+      <c r="I22" t="s">
+        <v>96</v>
+      </c>
+      <c r="J22" t="s">
+        <v>96</v>
+      </c>
+      <c r="K22" t="s">
+        <v>96</v>
+      </c>
+      <c r="L22" t="s">
+        <v>96</v>
+      </c>
+      <c r="M22" t="s">
+        <v>96</v>
+      </c>
+      <c r="N22" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="23" spans="8:20" x14ac:dyDescent="0.25">
+      <c r="H23" t="s">
+        <v>3</v>
+      </c>
+      <c r="I23" t="s">
+        <v>96</v>
+      </c>
+      <c r="J23" t="s">
+        <v>96</v>
+      </c>
+      <c r="K23" t="s">
+        <v>96</v>
+      </c>
+      <c r="L23" t="s">
+        <v>96</v>
+      </c>
+      <c r="M23" t="s">
+        <v>96</v>
+      </c>
+      <c r="N23" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="24" spans="8:20" x14ac:dyDescent="0.25">
+      <c r="H24" t="s">
+        <v>3</v>
+      </c>
+      <c r="I24" t="s">
+        <v>96</v>
+      </c>
+      <c r="J24" t="s">
+        <v>96</v>
+      </c>
+      <c r="K24" t="s">
+        <v>96</v>
+      </c>
+      <c r="L24" t="s">
+        <v>96</v>
+      </c>
+      <c r="M24" t="s">
+        <v>96</v>
+      </c>
+      <c r="N24" t="s">
+        <v>96</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -980,10 +1173,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G67"/>
+  <dimension ref="A1:L67"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -991,37 +1184,56 @@
     <col min="1" max="1" width="12.85546875" customWidth="1"/>
     <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="32.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="80.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D1" t="s">
         <v>78</v>
       </c>
-      <c r="C1" t="s">
-        <v>95</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F1" t="s">
+        <v>104</v>
+      </c>
+      <c r="G1">
+        <v>4</v>
+      </c>
+      <c r="H1" t="s">
+        <v>105</v>
+      </c>
+      <c r="I1">
+        <v>3</v>
+      </c>
+      <c r="J1" t="s">
+        <v>100</v>
+      </c>
+      <c r="K1">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
         <v>88</v>
       </c>
-      <c r="E1">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>89</v>
-      </c>
-      <c r="G1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>79</v>
       </c>
@@ -1032,12 +1244,12 @@
         <v>81</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>79</v>
       </c>
       <c r="C4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D4" t="s">
         <v>77</v>
@@ -1046,17 +1258,17 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>79</v>
       </c>
@@ -1067,12 +1279,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>79</v>
       </c>
       <c r="C8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D8" t="s">
         <v>77</v>
@@ -1081,17 +1293,17 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>79</v>
       </c>
@@ -1099,15 +1311,15 @@
         <v>80</v>
       </c>
       <c r="D11" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>79</v>
       </c>
       <c r="C12" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D12" t="s">
         <v>77</v>
@@ -1116,17 +1328,17 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>79</v>
       </c>
@@ -1134,15 +1346,15 @@
         <v>80</v>
       </c>
       <c r="D15" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>79</v>
+      </c>
+      <c r="C16" t="s">
         <v>84</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
-        <v>79</v>
-      </c>
-      <c r="C16" t="s">
-        <v>85</v>
       </c>
       <c r="D16" t="s">
         <v>77</v>
@@ -1151,17 +1363,17 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>79</v>
       </c>
@@ -1172,62 +1384,77 @@
         <v>77</v>
       </c>
       <c r="E19" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>79</v>
+      </c>
+      <c r="C20" t="s">
+        <v>94</v>
+      </c>
+      <c r="D20" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
-        <v>79</v>
-      </c>
-      <c r="C20" t="s">
-        <v>96</v>
-      </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>90</v>
+      </c>
+      <c r="B23" t="s">
+        <v>98</v>
+      </c>
+      <c r="C23" t="s">
+        <v>102</v>
+      </c>
+      <c r="D23" t="s">
+        <v>78</v>
+      </c>
+      <c r="E23" t="s">
+        <v>93</v>
+      </c>
+      <c r="F23" t="s">
         <v>86</v>
       </c>
-      <c r="E20" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>92</v>
-      </c>
-      <c r="B23" t="s">
-        <v>78</v>
-      </c>
-      <c r="C23" t="s">
-        <v>82</v>
-      </c>
-      <c r="D23" t="s">
+      <c r="G23">
+        <v>4</v>
+      </c>
+      <c r="H23" t="s">
+        <v>87</v>
+      </c>
+      <c r="I23">
+        <v>3</v>
+      </c>
+      <c r="J23" t="s">
+        <v>100</v>
+      </c>
+      <c r="K23">
+        <v>1</v>
+      </c>
+      <c r="L23" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
         <v>88</v>
       </c>
-      <c r="E23">
-        <v>4</v>
-      </c>
-      <c r="F23" t="s">
-        <v>89</v>
-      </c>
-      <c r="G23">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>79</v>
       </c>
@@ -1238,7 +1465,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>79</v>
       </c>
@@ -1252,17 +1479,17 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>79</v>
       </c>
@@ -1273,12 +1500,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>79</v>
       </c>
       <c r="C30" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D30" t="s">
         <v>77</v>
@@ -1287,17 +1514,17 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>79</v>
       </c>
@@ -1305,15 +1532,15 @@
         <v>80</v>
       </c>
       <c r="D33" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>79</v>
       </c>
       <c r="C34" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D34" t="s">
         <v>77</v>
@@ -1322,17 +1549,17 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>79</v>
       </c>
@@ -1340,34 +1567,34 @@
         <v>80</v>
       </c>
       <c r="D37" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>79</v>
+      </c>
+      <c r="C38" t="s">
         <v>84</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B38" t="s">
-        <v>79</v>
-      </c>
-      <c r="C38" t="s">
-        <v>85</v>
       </c>
       <c r="D38" t="s">
         <v>77</v>
       </c>
       <c r="E38" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>79</v>
       </c>
@@ -1378,10 +1605,10 @@
         <v>77</v>
       </c>
       <c r="E41" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
         <v>79</v>
       </c>
@@ -1395,45 +1622,60 @@
         <v>3</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>90</v>
+      </c>
+      <c r="B45" t="s">
+        <v>98</v>
+      </c>
+      <c r="C45" t="s">
+        <v>103</v>
+      </c>
+      <c r="D45" t="s">
+        <v>78</v>
+      </c>
+      <c r="E45" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>92</v>
-      </c>
-      <c r="B45" t="s">
-        <v>78</v>
-      </c>
-      <c r="C45" t="s">
-        <v>82</v>
-      </c>
-      <c r="D45" t="s">
+      <c r="F45" t="s">
+        <v>86</v>
+      </c>
+      <c r="G45">
+        <v>4</v>
+      </c>
+      <c r="H45" t="s">
+        <v>87</v>
+      </c>
+      <c r="I45">
+        <v>3</v>
+      </c>
+      <c r="J45" t="s">
+        <v>100</v>
+      </c>
+      <c r="K45">
+        <v>3</v>
+      </c>
+      <c r="L45" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
         <v>88</v>
       </c>
-      <c r="E45">
-        <v>4</v>
-      </c>
-      <c r="F45" t="s">
-        <v>89</v>
-      </c>
-      <c r="G45">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B46" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
         <v>79</v>
       </c>
@@ -1444,7 +1686,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
         <v>79</v>
       </c>
@@ -1460,12 +1702,12 @@
     </row>
     <row r="49" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="50" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="51" spans="2:5" x14ac:dyDescent="0.25">
@@ -1495,12 +1737,12 @@
     </row>
     <row r="53" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="54" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="55" spans="2:5" x14ac:dyDescent="0.25">
@@ -1511,7 +1753,7 @@
         <v>80</v>
       </c>
       <c r="D55" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="56" spans="2:5" x14ac:dyDescent="0.25">
@@ -1530,12 +1772,12 @@
     </row>
     <row r="57" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="58" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="59" spans="2:5" x14ac:dyDescent="0.25">
@@ -1546,7 +1788,7 @@
         <v>80</v>
       </c>
       <c r="D59" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="60" spans="2:5" x14ac:dyDescent="0.25">
@@ -1560,17 +1802,17 @@
         <v>77</v>
       </c>
       <c r="E60" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="61" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="62" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="63" spans="2:5" x14ac:dyDescent="0.25">
@@ -1584,7 +1826,7 @@
         <v>77</v>
       </c>
       <c r="E63" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="64" spans="2:5" x14ac:dyDescent="0.25">
@@ -1592,10 +1834,10 @@
         <v>79</v>
       </c>
       <c r="C64" t="s">
+        <v>84</v>
+      </c>
+      <c r="D64" t="s">
         <v>85</v>
-      </c>
-      <c r="D64" t="s">
-        <v>86</v>
       </c>
       <c r="E64" t="s">
         <v>3</v>
@@ -1603,17 +1845,17 @@
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
#5 added delay of the animation into the excel, source code updated
</commit_message>
<xml_diff>
--- a/colony.xlsx
+++ b/colony.xlsx
@@ -9,12 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13485" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13485"/>
   </bookViews>
   <sheets>
-    <sheet name="Environment_rules" sheetId="3" r:id="rId1"/>
-    <sheet name="Parameters" sheetId="1" r:id="rId2"/>
-    <sheet name="Environment" sheetId="2" r:id="rId3"/>
+    <sheet name="Parameters" sheetId="1" r:id="rId1"/>
+    <sheet name="Environment" sheetId="2" r:id="rId2"/>
+    <sheet name="Environment_rules" sheetId="3" r:id="rId3"/>
     <sheet name="Agents" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="107">
   <si>
     <t>environment rows</t>
   </si>
@@ -340,6 +340,9 @@
   </si>
   <si>
     <t>start j (-1 for random value)</t>
+  </si>
+  <si>
+    <t>animation delay, pause between displaying new iteration in seconds</t>
   </si>
 </sst>
 </file>
@@ -658,43 +661,56 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="63.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>95</v>
+      </c>
+      <c r="B4">
         <v>5</v>
       </c>
-      <c r="B1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" t="s">
-        <v>77</v>
-      </c>
-      <c r="C2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" t="s">
-        <v>77</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>106</v>
+      </c>
+      <c r="B5">
+        <v>0.91500000000000004</v>
       </c>
     </row>
   </sheetData>
@@ -703,57 +719,6 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="47.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>95</v>
-      </c>
-      <c r="B4">
-        <v>5</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T24"/>
   <sheetViews>
@@ -1171,12 +1136,58 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L67"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K45" sqref="K45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1222,7 +1233,7 @@
         <v>100</v>
       </c>
       <c r="K1">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="L1" t="s">
         <v>101</v>
@@ -1664,7 +1675,7 @@
         <v>100</v>
       </c>
       <c r="K45">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L45" t="s">
         <v>101</v>

</xml_diff>